<commit_message>
SCE 2026-2028 WMP - 2
</commit_message>
<xml_diff>
--- a/WMP26/SCE/SCE_PspsEventDamagePoint_2024.xlsx
+++ b/WMP26/SCE/SCE_PspsEventDamagePoint_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwm/Work/WEEDS/Calculations/Workpapers/WMP26/SCE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F775873-F060-8B48-A319-11CD05CB041A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FAC5ED-A500-3E4F-8393-8099E70A7DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="2120" windowWidth="30180" windowHeight="10840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="-15280" windowWidth="30180" windowHeight="10840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCE_PspsEventDamagePoint_2024" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,6 +395,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1354,7 +1355,7 @@
       <c r="P2" t="s">
         <v>51</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="10">
         <v>61.08</v>
       </c>
       <c r="R2">
@@ -1414,7 +1415,7 @@
       <c r="P3" t="s">
         <v>56</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="10">
         <v>62.18</v>
       </c>
       <c r="R3">
@@ -1474,7 +1475,7 @@
       <c r="P4" t="s">
         <v>60</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="10">
         <v>61.81</v>
       </c>
       <c r="R4">
@@ -1534,7 +1535,7 @@
       <c r="P5" t="s">
         <v>64</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="10">
         <v>76.41</v>
       </c>
       <c r="R5">
@@ -1594,7 +1595,7 @@
       <c r="P6" t="s">
         <v>68</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="10">
         <v>54.29</v>
       </c>
       <c r="R6">
@@ -1654,7 +1655,7 @@
       <c r="P7" t="s">
         <v>70</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="10">
         <v>51.07</v>
       </c>
       <c r="R7">
@@ -1714,7 +1715,7 @@
       <c r="P8" t="s">
         <v>72</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="10">
         <v>72.989999999999995</v>
       </c>
       <c r="R8">
@@ -1774,7 +1775,7 @@
       <c r="P9" t="s">
         <v>74</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="10">
         <v>44.86</v>
       </c>
       <c r="R9">
@@ -1834,7 +1835,7 @@
       <c r="P10" t="s">
         <v>76</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="10">
         <v>44.57</v>
       </c>
       <c r="R10">
@@ -1894,7 +1895,7 @@
       <c r="P11" t="s">
         <v>78</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="10">
         <v>68.83</v>
       </c>
       <c r="R11">
@@ -1954,7 +1955,7 @@
       <c r="P12" t="s">
         <v>54</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="10">
         <v>44.88</v>
       </c>
       <c r="R12">
@@ -2014,7 +2015,7 @@
       <c r="P13" t="s">
         <v>58</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="10">
         <v>73.58</v>
       </c>
       <c r="R13">
@@ -2071,7 +2072,7 @@
       <c r="P14" t="s">
         <v>63</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="10">
         <v>81.36</v>
       </c>
       <c r="R14">
@@ -2128,7 +2129,7 @@
       <c r="P15" t="s">
         <v>66</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="10">
         <v>64.66</v>
       </c>
       <c r="R15">

</xml_diff>